<commit_message>
- added config folder
</commit_message>
<xml_diff>
--- a/output/excel_output.xlsx
+++ b/output/excel_output.xlsx
@@ -122,7 +122,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>7480400.0</v>
+        <v>7478600.0</v>
       </c>
       <c r="C2" t="n">
         <v>32136.0</v>
@@ -139,10 +139,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>7579900.0</v>
+        <v>7504200.0</v>
       </c>
       <c r="C3" t="n">
-        <v>96008.0</v>
+        <v>32104.0</v>
       </c>
       <c r="D3" t="n">
         <v>849280.0</v>
@@ -156,7 +156,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>1279800.0</v>
+        <v>1295500.0</v>
       </c>
       <c r="C4" t="n">
         <v>1194848.0</v>
@@ -173,10 +173,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>126300.0</v>
+        <v>68500.0</v>
       </c>
       <c r="C5" t="n">
-        <v>64064.0</v>
+        <v>32128.0</v>
       </c>
       <c r="D5" t="n">
         <v>2013.0</v>
@@ -190,10 +190,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>3679500.0</v>
+        <v>2801600.0</v>
       </c>
       <c r="C6" t="n">
-        <v>1028096.0</v>
+        <v>32128.0</v>
       </c>
       <c r="D6" t="n">
         <v>3759.0</v>
@@ -207,16 +207,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>2178600.0</v>
+        <v>1733500.0</v>
       </c>
       <c r="C7" t="n">
         <v>32160.0</v>
       </c>
       <c r="D7" t="n">
-        <v>24900.0</v>
+        <v>23262.0</v>
       </c>
       <c r="E7" t="n">
-        <v>6300.0</v>
+        <v>5754.0</v>
       </c>
     </row>
     <row r="8">
@@ -224,7 +224,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>6965300.0</v>
+        <v>4301100.0</v>
       </c>
       <c r="C8" t="n">
         <v>32160.0</v>
@@ -268,7 +268,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>1.733145E8</v>
+        <v>1.786471E8</v>
       </c>
       <c r="C2" t="n">
         <v>320136.0</v>
@@ -285,10 +285,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>1.171914E8</v>
+        <v>1.895549E8</v>
       </c>
       <c r="C3" t="n">
-        <v>960008.0</v>
+        <v>320104.0</v>
       </c>
       <c r="D3" t="n">
         <v>8.4952772E7</v>
@@ -302,7 +302,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>2192700.0</v>
+        <v>3896100.0</v>
       </c>
       <c r="C4" t="n">
         <v>1.6191328E7</v>
@@ -319,10 +319,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>585300.0</v>
+        <v>1034700.0</v>
       </c>
       <c r="C5" t="n">
-        <v>640064.0</v>
+        <v>320128.0</v>
       </c>
       <c r="D5" t="n">
         <v>22022.0</v>
@@ -336,10 +336,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>4.00852E7</v>
+        <v>1.737307E8</v>
       </c>
       <c r="C6" t="n">
-        <v>1.0244096E7</v>
+        <v>320128.0</v>
       </c>
       <c r="D6" t="n">
         <v>45756.0</v>
@@ -353,16 +353,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>3920000.0</v>
+        <v>3305900.0</v>
       </c>
       <c r="C7" t="n">
         <v>320160.0</v>
       </c>
       <c r="D7" t="n">
-        <v>308226.0</v>
+        <v>325920.0</v>
       </c>
       <c r="E7" t="n">
-        <v>80742.0</v>
+        <v>86640.0</v>
       </c>
     </row>
     <row r="8">
@@ -370,7 +370,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>1.362752E8</v>
+        <v>1.132043E8</v>
       </c>
       <c r="C8" t="n">
         <v>320160.0</v>
@@ -414,7 +414,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>7133412.0</v>
+        <v>-4.23809488E8</v>
       </c>
       <c r="C2" t="n">
         <v>3200136.0</v>
@@ -431,10 +431,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>1.115408408E9</v>
+        <v>1.112973612E9</v>
       </c>
       <c r="C3" t="n">
-        <v>9600008.0</v>
+        <v>3200104.0</v>
       </c>
       <c r="D3" t="n">
         <v>8.458252322E9</v>
@@ -448,7 +448,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>8705700.0</v>
+        <v>1.17166E7</v>
       </c>
       <c r="C4" t="n">
         <v>2.04404192E8</v>
@@ -465,10 +465,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>2515600.0</v>
+        <v>3169000.0</v>
       </c>
       <c r="C5" t="n">
-        <v>6400064.0</v>
+        <v>3200128.0</v>
       </c>
       <c r="D5" t="n">
         <v>222034.0</v>
@@ -482,10 +482,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>1.8438632E9</v>
+        <v>-1.426433696E9</v>
       </c>
       <c r="C6" t="n">
-        <v>1.02404096E8</v>
+        <v>3200128.0</v>
       </c>
       <c r="D6" t="n">
         <v>345750.0</v>
@@ -499,16 +499,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>8758600.0</v>
+        <v>1.27537E7</v>
       </c>
       <c r="C7" t="n">
         <v>3200160.0</v>
       </c>
       <c r="D7" t="n">
-        <v>3784665.0</v>
+        <v>4000593.0</v>
       </c>
       <c r="E7" t="n">
-        <v>1039555.0</v>
+        <v>1111531.0</v>
       </c>
     </row>
     <row r="8">
@@ -516,7 +516,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-8.83080596E8</v>
+        <v>1.349283904E9</v>
       </c>
       <c r="C8" t="n">
         <v>3200160.0</v>
@@ -560,7 +560,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>554300.0</v>
+        <v>1513600.0</v>
       </c>
       <c r="C2" t="n">
         <v>32136.0</v>
@@ -577,10 +577,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>572200.0</v>
+        <v>2033900.0</v>
       </c>
       <c r="C3" t="n">
-        <v>96008.0</v>
+        <v>32104.0</v>
       </c>
       <c r="D3" t="n">
         <v>8.458755624E9</v>
@@ -594,7 +594,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>63600.0</v>
+        <v>165600.0</v>
       </c>
       <c r="C4" t="n">
         <v>1257184.0</v>
@@ -614,7 +614,7 @@
         <v>9400.0</v>
       </c>
       <c r="C5" t="n">
-        <v>64064.0</v>
+        <v>32128.0</v>
       </c>
       <c r="D5" t="n">
         <v>224040.0</v>
@@ -628,10 +628,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>143400.0</v>
+        <v>348500.0</v>
       </c>
       <c r="C6" t="n">
-        <v>1028096.0</v>
+        <v>32128.0</v>
       </c>
       <c r="D6" t="n">
         <v>349329.0</v>
@@ -645,16 +645,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>93300.0</v>
+        <v>225100.0</v>
       </c>
       <c r="C7" t="n">
         <v>32160.0</v>
       </c>
       <c r="D7" t="n">
-        <v>3807267.0</v>
+        <v>4020549.0</v>
       </c>
       <c r="E7" t="n">
-        <v>1045089.0</v>
+        <v>1116183.0</v>
       </c>
     </row>
     <row r="8">
@@ -662,7 +662,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>397200.0</v>
+        <v>1053500.0</v>
       </c>
       <c r="C8" t="n">
         <v>32160.0</v>
@@ -706,7 +706,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>6.66424E7</v>
+        <v>1.576722E8</v>
       </c>
       <c r="C2" t="n">
         <v>320136.0</v>
@@ -723,10 +723,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>6.90555E7</v>
+        <v>1.571949E8</v>
       </c>
       <c r="C3" t="n">
-        <v>960008.0</v>
+        <v>320104.0</v>
       </c>
       <c r="D3" t="n">
         <v>8.508377774E9</v>
@@ -740,7 +740,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>714300.0</v>
+        <v>1907500.0</v>
       </c>
       <c r="C4" t="n">
         <v>1.68696E7</v>
@@ -757,10 +757,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>120800.0</v>
+        <v>109100.0</v>
       </c>
       <c r="C5" t="n">
-        <v>640064.0</v>
+        <v>320128.0</v>
       </c>
       <c r="D5" t="n">
         <v>244049.0</v>
@@ -774,10 +774,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>1.299E7</v>
+        <v>3.40661E7</v>
       </c>
       <c r="C6" t="n">
-        <v>1.0244096E7</v>
+        <v>320128.0</v>
       </c>
       <c r="D6" t="n">
         <v>383709.0</v>
@@ -791,16 +791,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>996400.0</v>
+        <v>2505900.0</v>
       </c>
       <c r="C7" t="n">
         <v>320160.0</v>
       </c>
       <c r="D7" t="n">
-        <v>4101531.0</v>
+        <v>4317285.0</v>
       </c>
       <c r="E7" t="n">
-        <v>1123177.0</v>
+        <v>1195095.0</v>
       </c>
     </row>
     <row r="8">
@@ -808,7 +808,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>3.48716E7</v>
+        <v>7.78859E7</v>
       </c>
       <c r="C8" t="n">
         <v>320160.0</v>
@@ -852,7 +852,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>-1.400311588E9</v>
+        <v>-1.40086548E9</v>
       </c>
       <c r="C2" t="n">
         <v>3200136.0</v>
@@ -869,10 +869,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>5.8299308E7</v>
+        <v>7.81544112E8</v>
       </c>
       <c r="C3" t="n">
-        <v>9600008.0</v>
+        <v>3200104.0</v>
       </c>
       <c r="D3" t="n">
         <v>1.349985455E10</v>
@@ -886,7 +886,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>1.02521E7</v>
+        <v>1.31726E7</v>
       </c>
       <c r="C4" t="n">
         <v>2.11202912E8</v>
@@ -903,10 +903,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>119200.0</v>
+        <v>241500.0</v>
       </c>
       <c r="C5" t="n">
-        <v>6400064.0</v>
+        <v>3200128.0</v>
       </c>
       <c r="D5" t="n">
         <v>444053.0</v>
@@ -920,10 +920,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>1.306409E9</v>
+        <v>2.0379125E9</v>
       </c>
       <c r="C6" t="n">
-        <v>1.02404096E8</v>
+        <v>3200128.0</v>
       </c>
       <c r="D6" t="n">
         <v>730500.0</v>
@@ -937,16 +937,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>1.13355E7</v>
+        <v>1.78272E7</v>
       </c>
       <c r="C7" t="n">
         <v>3200160.0</v>
       </c>
       <c r="D7" t="n">
-        <v>7747038.0</v>
+        <v>8014272.0</v>
       </c>
       <c r="E7" t="n">
-        <v>2138346.0</v>
+        <v>2227424.0</v>
       </c>
     </row>
     <row r="8">
@@ -954,7 +954,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-8.16180796E8</v>
+        <v>1.528776804E9</v>
       </c>
       <c r="C8" t="n">
         <v>3200160.0</v>
@@ -998,7 +998,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>420500.0</v>
+        <v>583400.0</v>
       </c>
       <c r="C2" t="n">
         <v>32136.0</v>
@@ -1015,10 +1015,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>219700.0</v>
+        <v>283100.0</v>
       </c>
       <c r="C3" t="n">
-        <v>96008.0</v>
+        <v>32104.0</v>
       </c>
       <c r="D3" t="n">
         <v>1.3500011458E10</v>
@@ -1032,7 +1032,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>56500.0</v>
+        <v>102600.0</v>
       </c>
       <c r="C4" t="n">
         <v>1317728.0</v>
@@ -1049,10 +1049,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>1200.0</v>
+        <v>1900.0</v>
       </c>
       <c r="C5" t="n">
-        <v>64064.0</v>
+        <v>32128.0</v>
       </c>
       <c r="D5" t="n">
         <v>446051.0</v>
@@ -1066,10 +1066,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>5158700.0</v>
+        <v>3349800.0</v>
       </c>
       <c r="C6" t="n">
-        <v>1028096.0</v>
+        <v>32128.0</v>
       </c>
       <c r="D6" t="n">
         <v>733497.0</v>
@@ -1083,16 +1083,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>102200.0</v>
+        <v>153300.0</v>
       </c>
       <c r="C7" t="n">
         <v>32160.0</v>
       </c>
       <c r="D7" t="n">
-        <v>7770177.0</v>
+        <v>8035692.0</v>
       </c>
       <c r="E7" t="n">
-        <v>2144059.0</v>
+        <v>2232564.0</v>
       </c>
     </row>
     <row r="8">
@@ -1100,7 +1100,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>357700.0</v>
+        <v>580900.0</v>
       </c>
       <c r="C8" t="n">
         <v>32160.0</v>
@@ -1144,7 +1144,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>3.56385E7</v>
+        <v>4.98338E7</v>
       </c>
       <c r="C2" t="n">
         <v>320136.0</v>
@@ -1161,10 +1161,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>2.14231E7</v>
+        <v>3.49988E7</v>
       </c>
       <c r="C3" t="n">
-        <v>960008.0</v>
+        <v>320104.0</v>
       </c>
       <c r="D3" t="n">
         <v>1.3516300758E10</v>
@@ -1178,7 +1178,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>731900.0</v>
+        <v>1397300.0</v>
       </c>
       <c r="C4" t="n">
         <v>1.756656E7</v>
@@ -1195,10 +1195,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>11600.0</v>
+        <v>46300.0</v>
       </c>
       <c r="C5" t="n">
-        <v>640064.0</v>
+        <v>320128.0</v>
       </c>
       <c r="D5" t="n">
         <v>466049.0</v>
@@ -1212,10 +1212,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>3.93098E7</v>
+        <v>5.90093E7</v>
       </c>
       <c r="C6" t="n">
-        <v>1.0244096E7</v>
+        <v>320128.0</v>
       </c>
       <c r="D6" t="n">
         <v>763494.0</v>
@@ -1229,16 +1229,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>872300.0</v>
+        <v>2109400.0</v>
       </c>
       <c r="C7" t="n">
         <v>320160.0</v>
       </c>
       <c r="D7" t="n">
-        <v>8037393.0</v>
+        <v>8328342.0</v>
       </c>
       <c r="E7" t="n">
-        <v>2213131.0</v>
+        <v>2310114.0</v>
       </c>
     </row>
     <row r="8">
@@ -1246,7 +1246,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>3.46899E7</v>
+        <v>6.70331E7</v>
       </c>
       <c r="C8" t="n">
         <v>320160.0</v>
@@ -1290,7 +1290,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>9.77082004E8</v>
+        <v>-3.45289692E8</v>
       </c>
       <c r="C2" t="n">
         <v>3200136.0</v>
@@ -1307,10 +1307,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>2.097508E9</v>
+        <v>-7.49845396E8</v>
       </c>
       <c r="C3" t="n">
-        <v>9600008.0</v>
+        <v>3200104.0</v>
       </c>
       <c r="D3" t="n">
         <v>1.5148435334E10</v>
@@ -1324,7 +1324,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>7439900.0</v>
+        <v>1.54072E7</v>
       </c>
       <c r="C4" t="n">
         <v>2.18477152E8</v>
@@ -1341,10 +1341,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>119200.0</v>
+        <v>215100.0</v>
       </c>
       <c r="C5" t="n">
-        <v>6400064.0</v>
+        <v>3200128.0</v>
       </c>
       <c r="D5" t="n">
         <v>666047.0</v>
@@ -1358,10 +1358,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>1.9042218E9</v>
+        <v>-7.14967496E8</v>
       </c>
       <c r="C6" t="n">
-        <v>1.02404096E8</v>
+        <v>3200128.0</v>
       </c>
       <c r="D6" t="n">
         <v>1063491.0</v>
@@ -1375,16 +1375,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>8764400.0</v>
+        <v>1.22405E7</v>
       </c>
       <c r="C7" t="n">
         <v>3200160.0</v>
       </c>
       <c r="D7" t="n">
-        <v>1.1532027E7</v>
+        <v>1.1741022E7</v>
       </c>
       <c r="E7" t="n">
-        <v>3178009.0</v>
+        <v>3247674.0</v>
       </c>
     </row>
     <row r="8">
@@ -1392,7 +1392,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-8.39199196E8</v>
+        <v>1.557466204E9</v>
       </c>
       <c r="C8" t="n">
         <v>3200160.0</v>

</xml_diff>

<commit_message>
Bug fix, everything changed to long
</commit_message>
<xml_diff>
--- a/output/excel_output.xlsx
+++ b/output/excel_output.xlsx
@@ -122,7 +122,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>7480400.0</v>
+        <v>5339600.0</v>
       </c>
       <c r="C2" t="n">
         <v>32136.0</v>
@@ -139,10 +139,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>7579900.0</v>
+        <v>5461700.0</v>
       </c>
       <c r="C3" t="n">
-        <v>96008.0</v>
+        <v>32104.0</v>
       </c>
       <c r="D3" t="n">
         <v>849280.0</v>
@@ -156,7 +156,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>1279800.0</v>
+        <v>1178700.0</v>
       </c>
       <c r="C4" t="n">
         <v>1194848.0</v>
@@ -173,10 +173,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>126300.0</v>
+        <v>57000.0</v>
       </c>
       <c r="C5" t="n">
-        <v>64064.0</v>
+        <v>32128.0</v>
       </c>
       <c r="D5" t="n">
         <v>2013.0</v>
@@ -190,10 +190,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>3679500.0</v>
+        <v>2150100.0</v>
       </c>
       <c r="C6" t="n">
-        <v>1028096.0</v>
+        <v>32128.0</v>
       </c>
       <c r="D6" t="n">
         <v>3759.0</v>
@@ -207,16 +207,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>2178600.0</v>
+        <v>1406100.0</v>
       </c>
       <c r="C7" t="n">
         <v>32160.0</v>
       </c>
       <c r="D7" t="n">
-        <v>24900.0</v>
+        <v>19569.0</v>
       </c>
       <c r="E7" t="n">
-        <v>6300.0</v>
+        <v>4523.0</v>
       </c>
     </row>
     <row r="8">
@@ -224,7 +224,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>6965300.0</v>
+        <v>4206600.0</v>
       </c>
       <c r="C8" t="n">
         <v>32160.0</v>
@@ -268,7 +268,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>1.733145E8</v>
+        <v>1.017701E8</v>
       </c>
       <c r="C2" t="n">
         <v>320136.0</v>
@@ -285,10 +285,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>1.171914E8</v>
+        <v>7.90611E7</v>
       </c>
       <c r="C3" t="n">
-        <v>960008.0</v>
+        <v>320104.0</v>
       </c>
       <c r="D3" t="n">
         <v>8.4952772E7</v>
@@ -302,7 +302,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>2192700.0</v>
+        <v>2994500.0</v>
       </c>
       <c r="C4" t="n">
         <v>1.6191328E7</v>
@@ -319,10 +319,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>585300.0</v>
+        <v>521900.0</v>
       </c>
       <c r="C5" t="n">
-        <v>640064.0</v>
+        <v>320128.0</v>
       </c>
       <c r="D5" t="n">
         <v>22022.0</v>
@@ -336,10 +336,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>4.00852E7</v>
+        <v>8.30633E7</v>
       </c>
       <c r="C6" t="n">
-        <v>1.0244096E7</v>
+        <v>320128.0</v>
       </c>
       <c r="D6" t="n">
         <v>45756.0</v>
@@ -353,16 +353,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>3920000.0</v>
+        <v>2184800.0</v>
       </c>
       <c r="C7" t="n">
         <v>320160.0</v>
       </c>
       <c r="D7" t="n">
-        <v>308226.0</v>
+        <v>339711.0</v>
       </c>
       <c r="E7" t="n">
-        <v>80742.0</v>
+        <v>91237.0</v>
       </c>
     </row>
     <row r="8">
@@ -370,7 +370,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>1.362752E8</v>
+        <v>6.00103E7</v>
       </c>
       <c r="C8" t="n">
         <v>320160.0</v>
@@ -414,7 +414,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>7133412.0</v>
+        <v>9.3630357E9</v>
       </c>
       <c r="C2" t="n">
         <v>3200136.0</v>
@@ -431,10 +431,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>1.115408408E9</v>
+        <v>8.8135149E9</v>
       </c>
       <c r="C3" t="n">
-        <v>9600008.0</v>
+        <v>3200104.0</v>
       </c>
       <c r="D3" t="n">
         <v>8.458252322E9</v>
@@ -448,7 +448,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>8705700.0</v>
+        <v>1.05384E7</v>
       </c>
       <c r="C4" t="n">
         <v>2.04404192E8</v>
@@ -465,10 +465,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>2515600.0</v>
+        <v>3946400.0</v>
       </c>
       <c r="C5" t="n">
-        <v>6400064.0</v>
+        <v>3200128.0</v>
       </c>
       <c r="D5" t="n">
         <v>222034.0</v>
@@ -482,10 +482,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>1.8438632E9</v>
+        <v>2.2536142E9</v>
       </c>
       <c r="C6" t="n">
-        <v>1.02404096E8</v>
+        <v>3200128.0</v>
       </c>
       <c r="D6" t="n">
         <v>345750.0</v>
@@ -499,16 +499,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>8758600.0</v>
+        <v>1.4715E7</v>
       </c>
       <c r="C7" t="n">
         <v>3200160.0</v>
       </c>
       <c r="D7" t="n">
-        <v>3784665.0</v>
+        <v>3753264.0</v>
       </c>
       <c r="E7" t="n">
-        <v>1039555.0</v>
+        <v>1029088.0</v>
       </c>
     </row>
     <row r="8">
@@ -516,7 +516,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-8.83080596E8</v>
+        <v>4.3010016E9</v>
       </c>
       <c r="C8" t="n">
         <v>3200160.0</v>
@@ -560,7 +560,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>554300.0</v>
+        <v>622300.0</v>
       </c>
       <c r="C2" t="n">
         <v>32136.0</v>
@@ -577,10 +577,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>572200.0</v>
+        <v>860800.0</v>
       </c>
       <c r="C3" t="n">
-        <v>96008.0</v>
+        <v>32104.0</v>
       </c>
       <c r="D3" t="n">
         <v>8.458755624E9</v>
@@ -594,7 +594,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>63600.0</v>
+        <v>79300.0</v>
       </c>
       <c r="C4" t="n">
         <v>1257184.0</v>
@@ -611,10 +611,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>9400.0</v>
+        <v>3700.0</v>
       </c>
       <c r="C5" t="n">
-        <v>64064.0</v>
+        <v>32128.0</v>
       </c>
       <c r="D5" t="n">
         <v>224040.0</v>
@@ -628,10 +628,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>143400.0</v>
+        <v>143700.0</v>
       </c>
       <c r="C6" t="n">
-        <v>1028096.0</v>
+        <v>32128.0</v>
       </c>
       <c r="D6" t="n">
         <v>349329.0</v>
@@ -645,16 +645,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>93300.0</v>
+        <v>101200.0</v>
       </c>
       <c r="C7" t="n">
         <v>32160.0</v>
       </c>
       <c r="D7" t="n">
-        <v>3807267.0</v>
+        <v>3773814.0</v>
       </c>
       <c r="E7" t="n">
-        <v>1045089.0</v>
+        <v>1033938.0</v>
       </c>
     </row>
     <row r="8">
@@ -662,7 +662,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>397200.0</v>
+        <v>543200.0</v>
       </c>
       <c r="C8" t="n">
         <v>32160.0</v>
@@ -706,7 +706,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>6.66424E7</v>
+        <v>4.7413E7</v>
       </c>
       <c r="C2" t="n">
         <v>320136.0</v>
@@ -723,10 +723,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>6.90555E7</v>
+        <v>7.74947E7</v>
       </c>
       <c r="C3" t="n">
-        <v>960008.0</v>
+        <v>320104.0</v>
       </c>
       <c r="D3" t="n">
         <v>8.508377774E9</v>
@@ -740,7 +740,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>714300.0</v>
+        <v>1112200.0</v>
       </c>
       <c r="C4" t="n">
         <v>1.68696E7</v>
@@ -757,10 +757,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>120800.0</v>
+        <v>102200.0</v>
       </c>
       <c r="C5" t="n">
-        <v>640064.0</v>
+        <v>320128.0</v>
       </c>
       <c r="D5" t="n">
         <v>244049.0</v>
@@ -774,10 +774,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>1.299E7</v>
+        <v>1.50849E7</v>
       </c>
       <c r="C6" t="n">
-        <v>1.0244096E7</v>
+        <v>320128.0</v>
       </c>
       <c r="D6" t="n">
         <v>383709.0</v>
@@ -791,16 +791,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>996400.0</v>
+        <v>1204000.0</v>
       </c>
       <c r="C7" t="n">
         <v>320160.0</v>
       </c>
       <c r="D7" t="n">
-        <v>4101531.0</v>
+        <v>4102989.0</v>
       </c>
       <c r="E7" t="n">
-        <v>1123177.0</v>
+        <v>1123663.0</v>
       </c>
     </row>
     <row r="8">
@@ -808,7 +808,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>3.48716E7</v>
+        <v>5.14452E7</v>
       </c>
       <c r="C8" t="n">
         <v>320160.0</v>
@@ -852,7 +852,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>-1.400311588E9</v>
+        <v>1.47452185E10</v>
       </c>
       <c r="C2" t="n">
         <v>3200136.0</v>
@@ -869,10 +869,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>5.8299308E7</v>
+        <v>1.16304678E10</v>
       </c>
       <c r="C3" t="n">
-        <v>9600008.0</v>
+        <v>3200104.0</v>
       </c>
       <c r="D3" t="n">
         <v>1.349985455E10</v>
@@ -886,7 +886,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>1.02521E7</v>
+        <v>1.28222E7</v>
       </c>
       <c r="C4" t="n">
         <v>2.11202912E8</v>
@@ -903,10 +903,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>119200.0</v>
+        <v>90700.0</v>
       </c>
       <c r="C5" t="n">
-        <v>6400064.0</v>
+        <v>3200128.0</v>
       </c>
       <c r="D5" t="n">
         <v>444053.0</v>
@@ -920,10 +920,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>1.306409E9</v>
+        <v>1.6648463E9</v>
       </c>
       <c r="C6" t="n">
-        <v>1.02404096E8</v>
+        <v>3200128.0</v>
       </c>
       <c r="D6" t="n">
         <v>730500.0</v>
@@ -937,16 +937,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>1.13355E7</v>
+        <v>1.40566E7</v>
       </c>
       <c r="C7" t="n">
         <v>3200160.0</v>
       </c>
       <c r="D7" t="n">
-        <v>7747038.0</v>
+        <v>7639881.0</v>
       </c>
       <c r="E7" t="n">
-        <v>2138346.0</v>
+        <v>2102627.0</v>
       </c>
     </row>
     <row r="8">
@@ -954,7 +954,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-8.16180796E8</v>
+        <v>4.7138542E9</v>
       </c>
       <c r="C8" t="n">
         <v>3200160.0</v>
@@ -998,7 +998,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>420500.0</v>
+        <v>433500.0</v>
       </c>
       <c r="C2" t="n">
         <v>32136.0</v>
@@ -1015,10 +1015,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>219700.0</v>
+        <v>1092400.0</v>
       </c>
       <c r="C3" t="n">
-        <v>96008.0</v>
+        <v>32104.0</v>
       </c>
       <c r="D3" t="n">
         <v>1.3500011458E10</v>
@@ -1032,7 +1032,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>56500.0</v>
+        <v>88000.0</v>
       </c>
       <c r="C4" t="n">
         <v>1317728.0</v>
@@ -1049,10 +1049,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>1200.0</v>
+        <v>1400.0</v>
       </c>
       <c r="C5" t="n">
-        <v>64064.0</v>
+        <v>32128.0</v>
       </c>
       <c r="D5" t="n">
         <v>446051.0</v>
@@ -1066,10 +1066,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>5158700.0</v>
+        <v>4343600.0</v>
       </c>
       <c r="C6" t="n">
-        <v>1028096.0</v>
+        <v>32128.0</v>
       </c>
       <c r="D6" t="n">
         <v>733497.0</v>
@@ -1083,16 +1083,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>102200.0</v>
+        <v>116100.0</v>
       </c>
       <c r="C7" t="n">
         <v>32160.0</v>
       </c>
       <c r="D7" t="n">
-        <v>7770177.0</v>
+        <v>7663869.0</v>
       </c>
       <c r="E7" t="n">
-        <v>2144059.0</v>
+        <v>2108623.0</v>
       </c>
     </row>
     <row r="8">
@@ -1100,7 +1100,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>357700.0</v>
+        <v>556300.0</v>
       </c>
       <c r="C8" t="n">
         <v>32160.0</v>
@@ -1144,7 +1144,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>3.56385E7</v>
+        <v>3.67672E7</v>
       </c>
       <c r="C2" t="n">
         <v>320136.0</v>
@@ -1161,10 +1161,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>2.14231E7</v>
+        <v>1.87609E7</v>
       </c>
       <c r="C3" t="n">
-        <v>960008.0</v>
+        <v>320104.0</v>
       </c>
       <c r="D3" t="n">
         <v>1.3516300758E10</v>
@@ -1178,7 +1178,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>731900.0</v>
+        <v>1065500.0</v>
       </c>
       <c r="C4" t="n">
         <v>1.756656E7</v>
@@ -1195,10 +1195,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>11600.0</v>
+        <v>13100.0</v>
       </c>
       <c r="C5" t="n">
-        <v>640064.0</v>
+        <v>320128.0</v>
       </c>
       <c r="D5" t="n">
         <v>466049.0</v>
@@ -1212,10 +1212,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>3.93098E7</v>
+        <v>2.13561E7</v>
       </c>
       <c r="C6" t="n">
-        <v>1.0244096E7</v>
+        <v>320128.0</v>
       </c>
       <c r="D6" t="n">
         <v>763494.0</v>
@@ -1229,16 +1229,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>872300.0</v>
+        <v>965900.0</v>
       </c>
       <c r="C7" t="n">
         <v>320160.0</v>
       </c>
       <c r="D7" t="n">
-        <v>8037393.0</v>
+        <v>7958565.0</v>
       </c>
       <c r="E7" t="n">
-        <v>2213131.0</v>
+        <v>2186855.0</v>
       </c>
     </row>
     <row r="8">
@@ -1246,7 +1246,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>3.46899E7</v>
+        <v>4.5989E7</v>
       </c>
       <c r="C8" t="n">
         <v>320160.0</v>
@@ -1290,7 +1290,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>9.77082004E8</v>
+        <v>6.3090574E9</v>
       </c>
       <c r="C2" t="n">
         <v>3200136.0</v>
@@ -1307,10 +1307,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>2.097508E9</v>
+        <v>2.4952989E9</v>
       </c>
       <c r="C3" t="n">
-        <v>9600008.0</v>
+        <v>3200104.0</v>
       </c>
       <c r="D3" t="n">
         <v>1.5148435334E10</v>
@@ -1324,7 +1324,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>7439900.0</v>
+        <v>8964200.0</v>
       </c>
       <c r="C4" t="n">
         <v>2.18477152E8</v>
@@ -1341,10 +1341,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>119200.0</v>
+        <v>94200.0</v>
       </c>
       <c r="C5" t="n">
-        <v>6400064.0</v>
+        <v>3200128.0</v>
       </c>
       <c r="D5" t="n">
         <v>666047.0</v>
@@ -1358,10 +1358,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>1.9042218E9</v>
+        <v>2.1984571E9</v>
       </c>
       <c r="C6" t="n">
-        <v>1.02404096E8</v>
+        <v>3200128.0</v>
       </c>
       <c r="D6" t="n">
         <v>1063491.0</v>
@@ -1375,16 +1375,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>8764400.0</v>
+        <v>1.04662E7</v>
       </c>
       <c r="C7" t="n">
         <v>3200160.0</v>
       </c>
       <c r="D7" t="n">
-        <v>1.1532027E7</v>
+        <v>1.2150057E7</v>
       </c>
       <c r="E7" t="n">
-        <v>3178009.0</v>
+        <v>3384019.0</v>
       </c>
     </row>
     <row r="8">
@@ -1392,7 +1392,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-8.39199196E8</v>
+        <v>4.3251206E9</v>
       </c>
       <c r="C8" t="n">
         <v>3200160.0</v>

</xml_diff>